<commit_message>
More races and feats
</commit_message>
<xml_diff>
--- a/pathfinder-generator/src/main/resources/WeaponDatabase.xlsx
+++ b/pathfinder-generator/src/main/resources/WeaponDatabase.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/knichol/dev/personal/pathfinder-app/pathfinder-generator/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD40EE5-F2C2-1042-922C-8BB3E3AB9187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA628F05-C9B0-3242-852E-7ABF48A69380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18720" xr2:uid="{2BDF4080-FAE7-5142-9483-1187E643B50B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3343" uniqueCount="523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3331" uniqueCount="522">
   <si>
     <t>Name</t>
   </si>
@@ -1148,9 +1148,6 @@
     <t>B (or S)</t>
   </si>
   <si>
-    <t>Sabre, sawtoothAA1</t>
-  </si>
-  <si>
     <t>Sai</t>
   </si>
   <si>
@@ -1250,9 +1247,6 @@
     <t>Rhoka</t>
   </si>
   <si>
-    <t>Sabre, sawtoothAG</t>
-  </si>
-  <si>
     <t>Shotel</t>
   </si>
   <si>
@@ -1605,6 +1599,9 @@
   </si>
   <si>
     <t>Exotic</t>
+  </si>
+  <si>
+    <t>Sabre, sawtooth</t>
   </si>
 </sst>
 </file>
@@ -1965,10 +1962,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A30C0332-FD18-7F4B-8E91-B8280684E25C}">
-  <dimension ref="A1:L279"/>
+  <dimension ref="A1:L278"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="A201" sqref="A201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8132,7 +8129,7 @@
         <v>53</v>
       </c>
       <c r="L162" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="163" spans="1:12" x14ac:dyDescent="0.2">
@@ -8170,7 +8167,7 @@
         <v>53</v>
       </c>
       <c r="L163" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="164" spans="1:12" x14ac:dyDescent="0.2">
@@ -8208,7 +8205,7 @@
         <v>53</v>
       </c>
       <c r="L164" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="165" spans="1:12" x14ac:dyDescent="0.2">
@@ -8246,7 +8243,7 @@
         <v>53</v>
       </c>
       <c r="L165" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="166" spans="1:12" x14ac:dyDescent="0.2">
@@ -8284,7 +8281,7 @@
         <v>53</v>
       </c>
       <c r="L166" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="167" spans="1:12" x14ac:dyDescent="0.2">
@@ -8322,7 +8319,7 @@
         <v>53</v>
       </c>
       <c r="L167" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="168" spans="1:12" x14ac:dyDescent="0.2">
@@ -8360,7 +8357,7 @@
         <v>53</v>
       </c>
       <c r="L168" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="169" spans="1:12" x14ac:dyDescent="0.2">
@@ -8398,7 +8395,7 @@
         <v>53</v>
       </c>
       <c r="L169" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="170" spans="1:12" x14ac:dyDescent="0.2">
@@ -8436,7 +8433,7 @@
         <v>53</v>
       </c>
       <c r="L170" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="171" spans="1:12" x14ac:dyDescent="0.2">
@@ -8474,7 +8471,7 @@
         <v>53</v>
       </c>
       <c r="L171" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="172" spans="1:12" x14ac:dyDescent="0.2">
@@ -8512,7 +8509,7 @@
         <v>53</v>
       </c>
       <c r="L172" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="173" spans="1:12" x14ac:dyDescent="0.2">
@@ -8550,7 +8547,7 @@
         <v>53</v>
       </c>
       <c r="L173" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="174" spans="1:12" x14ac:dyDescent="0.2">
@@ -8588,7 +8585,7 @@
         <v>53</v>
       </c>
       <c r="L174" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="175" spans="1:12" x14ac:dyDescent="0.2">
@@ -8626,7 +8623,7 @@
         <v>53</v>
       </c>
       <c r="L175" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="176" spans="1:12" x14ac:dyDescent="0.2">
@@ -8664,7 +8661,7 @@
         <v>53</v>
       </c>
       <c r="L176" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="177" spans="1:12" x14ac:dyDescent="0.2">
@@ -8702,7 +8699,7 @@
         <v>53</v>
       </c>
       <c r="L177" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="178" spans="1:12" x14ac:dyDescent="0.2">
@@ -8740,7 +8737,7 @@
         <v>53</v>
       </c>
       <c r="L178" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="179" spans="1:12" x14ac:dyDescent="0.2">
@@ -8778,7 +8775,7 @@
         <v>53</v>
       </c>
       <c r="L179" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="180" spans="1:12" x14ac:dyDescent="0.2">
@@ -8786,37 +8783,37 @@
         <v>370</v>
       </c>
       <c r="B180" t="s">
-        <v>127</v>
+        <v>22</v>
       </c>
       <c r="C180" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D180" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="E180" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F180" t="s">
         <v>11</v>
       </c>
       <c r="G180" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="H180" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="I180" t="s">
-        <v>11</v>
+        <v>363</v>
       </c>
       <c r="J180" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="K180" t="s">
         <v>53</v>
       </c>
       <c r="L180" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="181" spans="1:12" x14ac:dyDescent="0.2">
@@ -8824,7 +8821,7 @@
         <v>371</v>
       </c>
       <c r="B181" t="s">
-        <v>22</v>
+        <v>372</v>
       </c>
       <c r="C181" t="s">
         <v>16</v>
@@ -8833,7 +8830,7 @@
         <v>8</v>
       </c>
       <c r="E181" t="s">
-        <v>10</v>
+        <v>165</v>
       </c>
       <c r="F181" t="s">
         <v>11</v>
@@ -8842,36 +8839,36 @@
         <v>19</v>
       </c>
       <c r="H181" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="I181" t="s">
-        <v>363</v>
+        <v>24</v>
       </c>
       <c r="J181" t="s">
-        <v>65</v>
+        <v>101</v>
       </c>
       <c r="K181" t="s">
         <v>53</v>
       </c>
       <c r="L181" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="182" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="B182" t="s">
-        <v>373</v>
+        <v>179</v>
       </c>
       <c r="C182" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D182" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E182" t="s">
-        <v>165</v>
+        <v>10</v>
       </c>
       <c r="F182" t="s">
         <v>11</v>
@@ -8880,19 +8877,19 @@
         <v>19</v>
       </c>
       <c r="H182" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="I182" t="s">
-        <v>24</v>
+        <v>73</v>
       </c>
       <c r="J182" t="s">
-        <v>101</v>
+        <v>65</v>
       </c>
       <c r="K182" t="s">
         <v>53</v>
       </c>
       <c r="L182" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="183" spans="1:12" x14ac:dyDescent="0.2">
@@ -8900,7 +8897,7 @@
         <v>374</v>
       </c>
       <c r="B183" t="s">
-        <v>179</v>
+        <v>31</v>
       </c>
       <c r="C183" t="s">
         <v>8</v>
@@ -8915,22 +8912,22 @@
         <v>11</v>
       </c>
       <c r="G183" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="H183" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I183" t="s">
-        <v>73</v>
+        <v>169</v>
       </c>
       <c r="J183" t="s">
-        <v>65</v>
+        <v>170</v>
       </c>
       <c r="K183" t="s">
         <v>53</v>
       </c>
       <c r="L183" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="184" spans="1:12" x14ac:dyDescent="0.2">
@@ -8938,7 +8935,7 @@
         <v>375</v>
       </c>
       <c r="B184" t="s">
-        <v>31</v>
+        <v>303</v>
       </c>
       <c r="C184" t="s">
         <v>8</v>
@@ -8953,22 +8950,22 @@
         <v>11</v>
       </c>
       <c r="G184" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="H184" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I184" t="s">
-        <v>169</v>
+        <v>11</v>
       </c>
       <c r="J184" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="K184" t="s">
         <v>53</v>
       </c>
       <c r="L184" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="185" spans="1:12" x14ac:dyDescent="0.2">
@@ -8976,7 +8973,7 @@
         <v>376</v>
       </c>
       <c r="B185" t="s">
-        <v>303</v>
+        <v>120</v>
       </c>
       <c r="C185" t="s">
         <v>8</v>
@@ -8985,28 +8982,28 @@
         <v>9</v>
       </c>
       <c r="E185" t="s">
-        <v>10</v>
+        <v>79</v>
       </c>
       <c r="F185" t="s">
         <v>11</v>
       </c>
       <c r="G185" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="H185" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="I185" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="J185" t="s">
-        <v>151</v>
+        <v>101</v>
       </c>
       <c r="K185" t="s">
         <v>53</v>
       </c>
       <c r="L185" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="186" spans="1:12" x14ac:dyDescent="0.2">
@@ -9014,7 +9011,7 @@
         <v>377</v>
       </c>
       <c r="B186" t="s">
-        <v>120</v>
+        <v>7</v>
       </c>
       <c r="C186" t="s">
         <v>8</v>
@@ -9023,19 +9020,19 @@
         <v>9</v>
       </c>
       <c r="E186" t="s">
-        <v>79</v>
+        <v>366</v>
       </c>
       <c r="F186" t="s">
         <v>11</v>
       </c>
       <c r="G186" t="s">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="H186" t="s">
         <v>20</v>
       </c>
       <c r="I186" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="J186" t="s">
         <v>101</v>
@@ -9044,7 +9041,7 @@
         <v>53</v>
       </c>
       <c r="L186" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="187" spans="1:12" x14ac:dyDescent="0.2">
@@ -9055,80 +9052,80 @@
         <v>7</v>
       </c>
       <c r="C187" t="s">
+        <v>16</v>
+      </c>
+      <c r="D187" t="s">
         <v>8</v>
       </c>
-      <c r="D187" t="s">
-        <v>9</v>
-      </c>
       <c r="E187" t="s">
-        <v>366</v>
+        <v>10</v>
       </c>
       <c r="F187" t="s">
         <v>11</v>
       </c>
       <c r="G187" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="H187" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="I187" t="s">
-        <v>24</v>
+        <v>379</v>
       </c>
       <c r="J187" t="s">
-        <v>101</v>
+        <v>170</v>
       </c>
       <c r="K187" t="s">
         <v>53</v>
       </c>
       <c r="L187" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="188" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B188" t="s">
-        <v>7</v>
+        <v>381</v>
       </c>
       <c r="C188" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D188" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="E188" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="F188" t="s">
         <v>11</v>
       </c>
       <c r="G188" t="s">
-        <v>54</v>
+        <v>148</v>
       </c>
       <c r="H188" t="s">
         <v>32</v>
       </c>
       <c r="I188" t="s">
-        <v>380</v>
+        <v>218</v>
       </c>
       <c r="J188" t="s">
-        <v>170</v>
+        <v>340</v>
       </c>
       <c r="K188" t="s">
-        <v>53</v>
+        <v>91</v>
       </c>
       <c r="L188" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="189" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="B189" t="s">
-        <v>382</v>
+        <v>221</v>
       </c>
       <c r="C189" t="s">
         <v>9</v>
@@ -9143,77 +9140,77 @@
         <v>11</v>
       </c>
       <c r="G189" t="s">
-        <v>148</v>
+        <v>383</v>
       </c>
       <c r="H189" t="s">
         <v>32</v>
       </c>
       <c r="I189" t="s">
-        <v>218</v>
+        <v>384</v>
       </c>
       <c r="J189" t="s">
-        <v>340</v>
+        <v>170</v>
       </c>
       <c r="K189" t="s">
         <v>91</v>
       </c>
       <c r="L189" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="190" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="B190" t="s">
-        <v>221</v>
+        <v>142</v>
       </c>
       <c r="C190" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="D190" t="s">
-        <v>56</v>
+        <v>121</v>
       </c>
       <c r="E190" t="s">
-        <v>34</v>
+        <v>165</v>
       </c>
       <c r="F190" t="s">
         <v>11</v>
       </c>
       <c r="G190" t="s">
-        <v>384</v>
+        <v>12</v>
       </c>
       <c r="H190" t="s">
-        <v>32</v>
+        <v>386</v>
       </c>
       <c r="I190" t="s">
-        <v>385</v>
+        <v>14</v>
       </c>
       <c r="J190" t="s">
-        <v>170</v>
+        <v>78</v>
       </c>
       <c r="K190" t="s">
         <v>91</v>
       </c>
       <c r="L190" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="191" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B191" t="s">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="C191" t="s">
-        <v>56</v>
+        <v>388</v>
       </c>
       <c r="D191" t="s">
-        <v>121</v>
+        <v>213</v>
       </c>
       <c r="E191" t="s">
-        <v>165</v>
+        <v>184</v>
       </c>
       <c r="F191" t="s">
         <v>11</v>
@@ -9222,36 +9219,36 @@
         <v>12</v>
       </c>
       <c r="H191" t="s">
-        <v>387</v>
+        <v>35</v>
       </c>
       <c r="I191" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="J191" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="K191" t="s">
         <v>91</v>
       </c>
       <c r="L191" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="192" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B192" t="s">
-        <v>120</v>
+        <v>272</v>
       </c>
       <c r="C192" t="s">
-        <v>389</v>
+        <v>9</v>
       </c>
       <c r="D192" t="s">
-        <v>213</v>
+        <v>56</v>
       </c>
       <c r="E192" t="s">
-        <v>184</v>
+        <v>390</v>
       </c>
       <c r="F192" t="s">
         <v>11</v>
@@ -9260,27 +9257,27 @@
         <v>12</v>
       </c>
       <c r="H192" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I192" t="s">
         <v>11</v>
       </c>
       <c r="J192" t="s">
-        <v>98</v>
+        <v>71</v>
       </c>
       <c r="K192" t="s">
         <v>91</v>
       </c>
       <c r="L192" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="193" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B193" t="s">
-        <v>272</v>
+        <v>221</v>
       </c>
       <c r="C193" t="s">
         <v>9</v>
@@ -9289,36 +9286,36 @@
         <v>56</v>
       </c>
       <c r="E193" t="s">
-        <v>391</v>
+        <v>10</v>
       </c>
       <c r="F193" t="s">
         <v>11</v>
       </c>
       <c r="G193" t="s">
-        <v>12</v>
+        <v>392</v>
       </c>
       <c r="H193" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="I193" t="s">
-        <v>11</v>
+        <v>258</v>
       </c>
       <c r="J193" t="s">
-        <v>71</v>
+        <v>393</v>
       </c>
       <c r="K193" t="s">
         <v>91</v>
       </c>
       <c r="L193" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="194" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="B194" t="s">
-        <v>221</v>
+        <v>257</v>
       </c>
       <c r="C194" t="s">
         <v>9</v>
@@ -9333,30 +9330,30 @@
         <v>11</v>
       </c>
       <c r="G194" t="s">
-        <v>393</v>
+        <v>59</v>
       </c>
       <c r="H194" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="I194" t="s">
-        <v>258</v>
+        <v>205</v>
       </c>
       <c r="J194" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="K194" t="s">
         <v>91</v>
       </c>
       <c r="L194" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="195" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B195" t="s">
-        <v>257</v>
+        <v>221</v>
       </c>
       <c r="C195" t="s">
         <v>9</v>
@@ -9365,28 +9362,28 @@
         <v>56</v>
       </c>
       <c r="E195" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F195" t="s">
         <v>11</v>
       </c>
       <c r="G195" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H195" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="I195" t="s">
-        <v>205</v>
+        <v>37</v>
       </c>
       <c r="J195" t="s">
-        <v>396</v>
+        <v>71</v>
       </c>
       <c r="K195" t="s">
         <v>91</v>
       </c>
       <c r="L195" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="196" spans="1:12" x14ac:dyDescent="0.2">
@@ -9394,37 +9391,37 @@
         <v>397</v>
       </c>
       <c r="B196" t="s">
-        <v>221</v>
+        <v>7</v>
       </c>
       <c r="C196" t="s">
+        <v>8</v>
+      </c>
+      <c r="D196" t="s">
         <v>9</v>
       </c>
-      <c r="D196" t="s">
-        <v>56</v>
-      </c>
       <c r="E196" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F196" t="s">
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="G196" t="s">
-        <v>57</v>
+        <v>12</v>
       </c>
       <c r="H196" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="I196" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="J196" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="K196" t="s">
         <v>91</v>
       </c>
       <c r="L196" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="197" spans="1:12" x14ac:dyDescent="0.2">
@@ -9432,37 +9429,37 @@
         <v>398</v>
       </c>
       <c r="B197" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
       <c r="C197" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D197" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="E197" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="F197" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="G197" t="s">
-        <v>12</v>
+        <v>148</v>
       </c>
       <c r="H197" t="s">
         <v>13</v>
       </c>
       <c r="I197" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="J197" t="s">
-        <v>82</v>
+        <v>340</v>
       </c>
       <c r="K197" t="s">
         <v>91</v>
       </c>
       <c r="L197" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="198" spans="1:12" x14ac:dyDescent="0.2">
@@ -9470,83 +9467,83 @@
         <v>399</v>
       </c>
       <c r="B198" t="s">
-        <v>158</v>
+        <v>400</v>
       </c>
       <c r="C198" t="s">
+        <v>8</v>
+      </c>
+      <c r="D198" t="s">
         <v>9</v>
       </c>
-      <c r="D198" t="s">
-        <v>56</v>
-      </c>
       <c r="E198" t="s">
-        <v>34</v>
+        <v>366</v>
       </c>
       <c r="F198" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G198" t="s">
-        <v>148</v>
+        <v>54</v>
       </c>
       <c r="H198" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="I198" t="s">
-        <v>11</v>
+        <v>401</v>
       </c>
       <c r="J198" t="s">
-        <v>340</v>
+        <v>101</v>
       </c>
       <c r="K198" t="s">
         <v>91</v>
       </c>
       <c r="L198" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="199" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="B199" t="s">
-        <v>401</v>
+        <v>7</v>
       </c>
       <c r="C199" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D199" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="E199" t="s">
-        <v>366</v>
+        <v>210</v>
       </c>
       <c r="F199" t="s">
         <v>11</v>
       </c>
       <c r="G199" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="H199" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I199" t="s">
-        <v>402</v>
+        <v>11</v>
       </c>
       <c r="J199" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="K199" t="s">
         <v>91</v>
       </c>
       <c r="L199" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="200" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>403</v>
+        <v>521</v>
       </c>
       <c r="B200" t="s">
-        <v>7</v>
+        <v>127</v>
       </c>
       <c r="C200" t="s">
         <v>9</v>
@@ -9555,13 +9552,13 @@
         <v>56</v>
       </c>
       <c r="E200" t="s">
-        <v>210</v>
+        <v>17</v>
       </c>
       <c r="F200" t="s">
         <v>11</v>
       </c>
       <c r="G200" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="H200" t="s">
         <v>32</v>
@@ -9570,21 +9567,21 @@
         <v>11</v>
       </c>
       <c r="J200" t="s">
-        <v>87</v>
+        <v>203</v>
       </c>
       <c r="K200" t="s">
         <v>91</v>
       </c>
       <c r="L200" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="201" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B201" t="s">
-        <v>127</v>
+        <v>303</v>
       </c>
       <c r="C201" t="s">
         <v>9</v>
@@ -9593,36 +9590,36 @@
         <v>56</v>
       </c>
       <c r="E201" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="F201" t="s">
         <v>11</v>
       </c>
       <c r="G201" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="H201" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I201" t="s">
-        <v>11</v>
+        <v>169</v>
       </c>
       <c r="J201" t="s">
-        <v>203</v>
+        <v>170</v>
       </c>
       <c r="K201" t="s">
         <v>91</v>
       </c>
       <c r="L201" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="202" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B202" t="s">
-        <v>303</v>
+        <v>221</v>
       </c>
       <c r="C202" t="s">
         <v>9</v>
@@ -9631,28 +9628,28 @@
         <v>56</v>
       </c>
       <c r="E202" t="s">
-        <v>34</v>
+        <v>165</v>
       </c>
       <c r="F202" t="s">
         <v>11</v>
       </c>
       <c r="G202" t="s">
-        <v>54</v>
+        <v>12</v>
       </c>
       <c r="H202" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I202" t="s">
-        <v>169</v>
+        <v>405</v>
       </c>
       <c r="J202" t="s">
-        <v>170</v>
+        <v>101</v>
       </c>
       <c r="K202" t="s">
         <v>91</v>
       </c>
       <c r="L202" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="203" spans="1:12" x14ac:dyDescent="0.2">
@@ -9660,22 +9657,22 @@
         <v>406</v>
       </c>
       <c r="B203" t="s">
-        <v>221</v>
+        <v>287</v>
       </c>
       <c r="C203" t="s">
-        <v>9</v>
+        <v>121</v>
       </c>
       <c r="D203" t="s">
-        <v>56</v>
+        <v>245</v>
       </c>
       <c r="E203" t="s">
-        <v>165</v>
+        <v>79</v>
       </c>
       <c r="F203" t="s">
         <v>11</v>
       </c>
       <c r="G203" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="H203" t="s">
         <v>32</v>
@@ -9684,13 +9681,13 @@
         <v>407</v>
       </c>
       <c r="J203" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="K203" t="s">
         <v>91</v>
       </c>
       <c r="L203" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="204" spans="1:12" x14ac:dyDescent="0.2">
@@ -9698,37 +9695,37 @@
         <v>408</v>
       </c>
       <c r="B204" t="s">
-        <v>287</v>
+        <v>221</v>
       </c>
       <c r="C204" t="s">
-        <v>121</v>
+        <v>9</v>
       </c>
       <c r="D204" t="s">
-        <v>245</v>
+        <v>56</v>
       </c>
       <c r="E204" t="s">
-        <v>79</v>
+        <v>17</v>
       </c>
       <c r="F204" t="s">
         <v>11</v>
       </c>
       <c r="G204" t="s">
-        <v>57</v>
+        <v>409</v>
       </c>
       <c r="H204" t="s">
         <v>32</v>
       </c>
       <c r="I204" t="s">
-        <v>409</v>
+        <v>11</v>
       </c>
       <c r="J204" t="s">
-        <v>78</v>
+        <v>203</v>
       </c>
       <c r="K204" t="s">
         <v>91</v>
       </c>
       <c r="L204" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="205" spans="1:12" x14ac:dyDescent="0.2">
@@ -9736,13 +9733,13 @@
         <v>410</v>
       </c>
       <c r="B205" t="s">
-        <v>221</v>
+        <v>127</v>
       </c>
       <c r="C205" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="D205" t="s">
-        <v>56</v>
+        <v>121</v>
       </c>
       <c r="E205" t="s">
         <v>17</v>
@@ -9751,7 +9748,7 @@
         <v>11</v>
       </c>
       <c r="G205" t="s">
-        <v>411</v>
+        <v>59</v>
       </c>
       <c r="H205" t="s">
         <v>32</v>
@@ -9760,97 +9757,97 @@
         <v>11</v>
       </c>
       <c r="J205" t="s">
-        <v>203</v>
+        <v>65</v>
       </c>
       <c r="K205" t="s">
         <v>91</v>
       </c>
       <c r="L205" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="206" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B206" t="s">
-        <v>127</v>
+        <v>272</v>
       </c>
       <c r="C206" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="D206" t="s">
-        <v>121</v>
+        <v>9</v>
       </c>
       <c r="E206" t="s">
-        <v>17</v>
+        <v>390</v>
       </c>
       <c r="F206" t="s">
         <v>11</v>
       </c>
       <c r="G206" t="s">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="H206" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I206" t="s">
         <v>11</v>
       </c>
       <c r="J206" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="K206" t="s">
         <v>91</v>
       </c>
       <c r="L206" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="207" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B207" t="s">
-        <v>272</v>
+        <v>303</v>
       </c>
       <c r="C207" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="D207" t="s">
-        <v>9</v>
+        <v>121</v>
       </c>
       <c r="E207" t="s">
-        <v>391</v>
+        <v>34</v>
       </c>
       <c r="F207" t="s">
         <v>11</v>
       </c>
       <c r="G207" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="H207" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I207" t="s">
         <v>11</v>
       </c>
       <c r="J207" t="s">
-        <v>98</v>
+        <v>65</v>
       </c>
       <c r="K207" t="s">
         <v>91</v>
       </c>
       <c r="L207" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="208" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B208" t="s">
-        <v>303</v>
+        <v>372</v>
       </c>
       <c r="C208" t="s">
         <v>56</v>
@@ -9865,60 +9862,60 @@
         <v>11</v>
       </c>
       <c r="G208" t="s">
-        <v>57</v>
+        <v>240</v>
       </c>
       <c r="H208" t="s">
         <v>32</v>
       </c>
       <c r="I208" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="J208" t="s">
-        <v>65</v>
+        <v>125</v>
       </c>
       <c r="K208" t="s">
         <v>91</v>
       </c>
       <c r="L208" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="209" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B209" t="s">
-        <v>373</v>
+        <v>22</v>
       </c>
       <c r="C209" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="D209" t="s">
-        <v>121</v>
+        <v>16</v>
       </c>
       <c r="E209" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="F209" t="s">
         <v>11</v>
       </c>
       <c r="G209" t="s">
-        <v>240</v>
+        <v>26</v>
       </c>
       <c r="H209" t="s">
         <v>32</v>
       </c>
       <c r="I209" t="s">
-        <v>14</v>
+        <v>415</v>
       </c>
       <c r="J209" t="s">
-        <v>125</v>
+        <v>65</v>
       </c>
       <c r="K209" t="s">
         <v>91</v>
       </c>
       <c r="L209" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="210" spans="1:12" x14ac:dyDescent="0.2">
@@ -9926,104 +9923,104 @@
         <v>416</v>
       </c>
       <c r="B210" t="s">
-        <v>22</v>
+        <v>372</v>
       </c>
       <c r="C210" t="s">
-        <v>23</v>
+        <v>105</v>
       </c>
       <c r="D210" t="s">
-        <v>16</v>
+        <v>417</v>
       </c>
       <c r="E210" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="F210" t="s">
         <v>11</v>
       </c>
       <c r="G210" t="s">
-        <v>26</v>
+        <v>418</v>
       </c>
       <c r="H210" t="s">
         <v>32</v>
       </c>
       <c r="I210" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="J210" t="s">
         <v>65</v>
       </c>
       <c r="K210" t="s">
-        <v>91</v>
+        <v>117</v>
       </c>
       <c r="L210" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="211" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="B211" t="s">
-        <v>373</v>
+        <v>421</v>
       </c>
       <c r="C211" t="s">
-        <v>105</v>
+        <v>253</v>
       </c>
       <c r="D211" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="E211" t="s">
-        <v>34</v>
+        <v>423</v>
       </c>
       <c r="F211" t="s">
         <v>11</v>
       </c>
       <c r="G211" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="H211" t="s">
         <v>32</v>
       </c>
       <c r="I211" t="s">
-        <v>421</v>
+        <v>14</v>
       </c>
       <c r="J211" t="s">
-        <v>65</v>
+        <v>101</v>
       </c>
       <c r="K211" t="s">
         <v>117</v>
       </c>
       <c r="L211" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="212" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="B212" t="s">
-        <v>423</v>
+        <v>221</v>
       </c>
       <c r="C212" t="s">
-        <v>253</v>
+        <v>104</v>
       </c>
       <c r="D212" t="s">
-        <v>424</v>
+        <v>105</v>
       </c>
       <c r="E212" t="s">
-        <v>425</v>
+        <v>10</v>
       </c>
       <c r="F212" t="s">
         <v>11</v>
       </c>
       <c r="G212" t="s">
-        <v>426</v>
+        <v>57</v>
       </c>
       <c r="H212" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="I212" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="J212" t="s">
         <v>101</v>
@@ -10032,15 +10029,15 @@
         <v>117</v>
       </c>
       <c r="L212" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="213" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B213" t="s">
-        <v>221</v>
+        <v>58</v>
       </c>
       <c r="C213" t="s">
         <v>104</v>
@@ -10058,10 +10055,10 @@
         <v>57</v>
       </c>
       <c r="H213" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="I213" t="s">
-        <v>37</v>
+        <v>427</v>
       </c>
       <c r="J213" t="s">
         <v>101</v>
@@ -10070,7 +10067,7 @@
         <v>117</v>
       </c>
       <c r="L213" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="214" spans="1:12" x14ac:dyDescent="0.2">
@@ -10078,7 +10075,7 @@
         <v>428</v>
       </c>
       <c r="B214" t="s">
-        <v>58</v>
+        <v>127</v>
       </c>
       <c r="C214" t="s">
         <v>104</v>
@@ -10087,16 +10084,16 @@
         <v>105</v>
       </c>
       <c r="E214" t="s">
-        <v>10</v>
+        <v>79</v>
       </c>
       <c r="F214" t="s">
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="G214" t="s">
         <v>57</v>
       </c>
       <c r="H214" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="I214" t="s">
         <v>429</v>
@@ -10108,7 +10105,7 @@
         <v>117</v>
       </c>
       <c r="L214" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="215" spans="1:12" x14ac:dyDescent="0.2">
@@ -10116,51 +10113,51 @@
         <v>430</v>
       </c>
       <c r="B215" t="s">
-        <v>127</v>
+        <v>158</v>
       </c>
       <c r="C215" t="s">
-        <v>104</v>
+        <v>9</v>
       </c>
       <c r="D215" t="s">
-        <v>105</v>
+        <v>213</v>
       </c>
       <c r="E215" t="s">
-        <v>79</v>
+        <v>10</v>
       </c>
       <c r="F215" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="G215" t="s">
-        <v>57</v>
+        <v>249</v>
       </c>
       <c r="H215" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="I215" t="s">
-        <v>431</v>
+        <v>205</v>
       </c>
       <c r="J215" t="s">
-        <v>101</v>
+        <v>65</v>
       </c>
       <c r="K215" t="s">
         <v>117</v>
       </c>
       <c r="L215" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="216" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B216" t="s">
-        <v>158</v>
+        <v>22</v>
       </c>
       <c r="C216" t="s">
+        <v>8</v>
+      </c>
+      <c r="D216" t="s">
         <v>9</v>
-      </c>
-      <c r="D216" t="s">
-        <v>213</v>
       </c>
       <c r="E216" t="s">
         <v>10</v>
@@ -10169,68 +10166,68 @@
         <v>11</v>
       </c>
       <c r="G216" t="s">
-        <v>249</v>
+        <v>148</v>
       </c>
       <c r="H216" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="I216" t="s">
-        <v>205</v>
+        <v>258</v>
       </c>
       <c r="J216" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="K216" t="s">
         <v>117</v>
       </c>
       <c r="L216" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="217" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B217" t="s">
-        <v>22</v>
+        <v>400</v>
       </c>
       <c r="C217" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="D217" t="s">
-        <v>9</v>
+        <v>121</v>
       </c>
       <c r="E217" t="s">
-        <v>10</v>
+        <v>184</v>
       </c>
       <c r="F217" t="s">
         <v>11</v>
       </c>
       <c r="G217" t="s">
-        <v>148</v>
+        <v>383</v>
       </c>
       <c r="H217" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="I217" t="s">
-        <v>258</v>
+        <v>11</v>
       </c>
       <c r="J217" t="s">
-        <v>98</v>
+        <v>65</v>
       </c>
       <c r="K217" t="s">
         <v>117</v>
       </c>
       <c r="L217" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="218" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B218" t="s">
-        <v>401</v>
+        <v>120</v>
       </c>
       <c r="C218" t="s">
         <v>56</v>
@@ -10239,28 +10236,28 @@
         <v>121</v>
       </c>
       <c r="E218" t="s">
-        <v>184</v>
+        <v>10</v>
       </c>
       <c r="F218" t="s">
         <v>11</v>
       </c>
       <c r="G218" t="s">
-        <v>384</v>
+        <v>418</v>
       </c>
       <c r="H218" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="I218" t="s">
-        <v>11</v>
+        <v>434</v>
       </c>
       <c r="J218" t="s">
-        <v>65</v>
+        <v>101</v>
       </c>
       <c r="K218" t="s">
         <v>117</v>
       </c>
       <c r="L218" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="219" spans="1:12" x14ac:dyDescent="0.2">
@@ -10268,92 +10265,92 @@
         <v>435</v>
       </c>
       <c r="B219" t="s">
-        <v>120</v>
+        <v>158</v>
       </c>
       <c r="C219" t="s">
-        <v>56</v>
+        <v>105</v>
       </c>
       <c r="D219" t="s">
-        <v>121</v>
+        <v>417</v>
       </c>
       <c r="E219" t="s">
-        <v>10</v>
+        <v>423</v>
       </c>
       <c r="F219" t="s">
         <v>11</v>
       </c>
       <c r="G219" t="s">
-        <v>420</v>
+        <v>240</v>
       </c>
       <c r="H219" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="I219" t="s">
-        <v>436</v>
+        <v>419</v>
       </c>
       <c r="J219" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="K219" t="s">
         <v>117</v>
       </c>
       <c r="L219" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="220" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B220" t="s">
-        <v>158</v>
+        <v>221</v>
       </c>
       <c r="C220" t="s">
-        <v>105</v>
+        <v>9</v>
       </c>
       <c r="D220" t="s">
-        <v>419</v>
+        <v>56</v>
       </c>
       <c r="E220" t="s">
-        <v>425</v>
+        <v>34</v>
       </c>
       <c r="F220" t="s">
         <v>11</v>
       </c>
       <c r="G220" t="s">
-        <v>240</v>
+        <v>249</v>
       </c>
       <c r="H220" t="s">
         <v>35</v>
       </c>
       <c r="I220" t="s">
-        <v>421</v>
+        <v>95</v>
       </c>
       <c r="J220" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="K220" t="s">
         <v>117</v>
       </c>
       <c r="L220" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="221" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B221" t="s">
-        <v>221</v>
+        <v>266</v>
       </c>
       <c r="C221" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="D221" t="s">
-        <v>56</v>
+        <v>121</v>
       </c>
       <c r="E221" t="s">
-        <v>34</v>
+        <v>210</v>
       </c>
       <c r="F221" t="s">
         <v>11</v>
@@ -10362,36 +10359,36 @@
         <v>249</v>
       </c>
       <c r="H221" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I221" t="s">
-        <v>95</v>
+        <v>258</v>
       </c>
       <c r="J221" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="K221" t="s">
         <v>117</v>
       </c>
       <c r="L221" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="222" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
+        <v>438</v>
+      </c>
+      <c r="B222" t="s">
         <v>439</v>
       </c>
-      <c r="B222" t="s">
-        <v>266</v>
-      </c>
       <c r="C222" t="s">
-        <v>56</v>
+        <v>105</v>
       </c>
       <c r="D222" t="s">
-        <v>121</v>
+        <v>417</v>
       </c>
       <c r="E222" t="s">
-        <v>210</v>
+        <v>10</v>
       </c>
       <c r="F222" t="s">
         <v>11</v>
@@ -10400,33 +10397,33 @@
         <v>249</v>
       </c>
       <c r="H222" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="I222" t="s">
-        <v>258</v>
+        <v>440</v>
       </c>
       <c r="J222" t="s">
-        <v>101</v>
+        <v>65</v>
       </c>
       <c r="K222" t="s">
         <v>117</v>
       </c>
       <c r="L222" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="223" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="B223" t="s">
-        <v>441</v>
+        <v>38</v>
       </c>
       <c r="C223" t="s">
-        <v>105</v>
+        <v>9</v>
       </c>
       <c r="D223" t="s">
-        <v>419</v>
+        <v>56</v>
       </c>
       <c r="E223" t="s">
         <v>10</v>
@@ -10444,13 +10441,13 @@
         <v>442</v>
       </c>
       <c r="J223" t="s">
-        <v>65</v>
+        <v>393</v>
       </c>
       <c r="K223" t="s">
         <v>117</v>
       </c>
       <c r="L223" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="224" spans="1:12" x14ac:dyDescent="0.2">
@@ -10458,37 +10455,37 @@
         <v>443</v>
       </c>
       <c r="B224" t="s">
-        <v>38</v>
+        <v>120</v>
       </c>
       <c r="C224" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="D224" t="s">
-        <v>56</v>
+        <v>121</v>
       </c>
       <c r="E224" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F224" t="s">
         <v>11</v>
       </c>
       <c r="G224" t="s">
-        <v>249</v>
+        <v>59</v>
       </c>
       <c r="H224" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="I224" t="s">
         <v>444</v>
       </c>
       <c r="J224" t="s">
-        <v>394</v>
+        <v>87</v>
       </c>
       <c r="K224" t="s">
         <v>117</v>
       </c>
       <c r="L224" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="225" spans="1:12" x14ac:dyDescent="0.2">
@@ -10496,22 +10493,22 @@
         <v>445</v>
       </c>
       <c r="B225" t="s">
-        <v>120</v>
+        <v>142</v>
       </c>
       <c r="C225" t="s">
-        <v>56</v>
+        <v>121</v>
       </c>
       <c r="D225" t="s">
-        <v>121</v>
+        <v>253</v>
       </c>
       <c r="E225" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="F225" t="s">
         <v>11</v>
       </c>
       <c r="G225" t="s">
-        <v>59</v>
+        <v>240</v>
       </c>
       <c r="H225" t="s">
         <v>32</v>
@@ -10520,13 +10517,13 @@
         <v>446</v>
       </c>
       <c r="J225" t="s">
-        <v>87</v>
+        <v>170</v>
       </c>
       <c r="K225" t="s">
         <v>117</v>
       </c>
       <c r="L225" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="226" spans="1:12" x14ac:dyDescent="0.2">
@@ -10534,22 +10531,22 @@
         <v>447</v>
       </c>
       <c r="B226" t="s">
-        <v>142</v>
+        <v>179</v>
       </c>
       <c r="C226" t="s">
-        <v>121</v>
+        <v>8</v>
       </c>
       <c r="D226" t="s">
-        <v>253</v>
+        <v>9</v>
       </c>
       <c r="E226" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="F226" t="s">
         <v>11</v>
       </c>
       <c r="G226" t="s">
-        <v>240</v>
+        <v>19</v>
       </c>
       <c r="H226" t="s">
         <v>32</v>
@@ -10558,13 +10555,13 @@
         <v>448</v>
       </c>
       <c r="J226" t="s">
-        <v>170</v>
+        <v>87</v>
       </c>
       <c r="K226" t="s">
         <v>117</v>
       </c>
       <c r="L226" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="227" spans="1:12" x14ac:dyDescent="0.2">
@@ -10572,113 +10569,113 @@
         <v>449</v>
       </c>
       <c r="B227" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="C227" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="D227" t="s">
-        <v>9</v>
+        <v>245</v>
       </c>
       <c r="E227" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="F227" t="s">
         <v>11</v>
       </c>
       <c r="G227" t="s">
-        <v>19</v>
+        <v>240</v>
       </c>
       <c r="H227" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="I227" t="s">
-        <v>450</v>
+        <v>95</v>
       </c>
       <c r="J227" t="s">
-        <v>87</v>
+        <v>340</v>
       </c>
       <c r="K227" t="s">
         <v>117</v>
       </c>
       <c r="L227" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="228" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
+        <v>450</v>
+      </c>
+      <c r="B228" t="s">
+        <v>221</v>
+      </c>
+      <c r="C228" t="s">
+        <v>113</v>
+      </c>
+      <c r="D228" t="s">
+        <v>114</v>
+      </c>
+      <c r="E228" t="s">
         <v>451</v>
       </c>
-      <c r="B228" t="s">
-        <v>158</v>
-      </c>
-      <c r="C228" t="s">
-        <v>56</v>
-      </c>
-      <c r="D228" t="s">
-        <v>245</v>
-      </c>
-      <c r="E228" t="s">
-        <v>34</v>
-      </c>
       <c r="F228" t="s">
         <v>11</v>
       </c>
       <c r="G228" t="s">
-        <v>240</v>
+        <v>59</v>
       </c>
       <c r="H228" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="I228" t="s">
-        <v>95</v>
+        <v>452</v>
       </c>
       <c r="J228" t="s">
-        <v>340</v>
+        <v>65</v>
       </c>
       <c r="K228" t="s">
         <v>117</v>
       </c>
       <c r="L228" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="229" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B229" t="s">
-        <v>221</v>
+        <v>7</v>
       </c>
       <c r="C229" t="s">
-        <v>113</v>
+        <v>9</v>
       </c>
       <c r="D229" t="s">
-        <v>114</v>
+        <v>56</v>
       </c>
       <c r="E229" t="s">
-        <v>453</v>
+        <v>34</v>
       </c>
       <c r="F229" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G229" t="s">
-        <v>59</v>
+        <v>454</v>
       </c>
       <c r="H229" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="I229" t="s">
-        <v>454</v>
+        <v>97</v>
       </c>
       <c r="J229" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="K229" t="s">
         <v>117</v>
       </c>
       <c r="L229" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="230" spans="1:12" x14ac:dyDescent="0.2">
@@ -10686,51 +10683,51 @@
         <v>455</v>
       </c>
       <c r="B230" t="s">
-        <v>7</v>
+        <v>120</v>
       </c>
       <c r="C230" t="s">
-        <v>9</v>
+        <v>121</v>
       </c>
       <c r="D230" t="s">
-        <v>56</v>
+        <v>253</v>
       </c>
       <c r="E230" t="s">
         <v>34</v>
       </c>
       <c r="F230" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G230" t="s">
-        <v>456</v>
+        <v>237</v>
       </c>
       <c r="H230" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I230" t="s">
-        <v>97</v>
+        <v>176</v>
       </c>
       <c r="J230" t="s">
-        <v>72</v>
+        <v>125</v>
       </c>
       <c r="K230" t="s">
         <v>117</v>
       </c>
       <c r="L230" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="231" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B231" t="s">
-        <v>120</v>
+        <v>39</v>
       </c>
       <c r="C231" t="s">
         <v>121</v>
       </c>
       <c r="D231" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="E231" t="s">
         <v>34</v>
@@ -10739,10 +10736,10 @@
         <v>11</v>
       </c>
       <c r="G231" t="s">
-        <v>237</v>
+        <v>457</v>
       </c>
       <c r="H231" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="I231" t="s">
         <v>176</v>
@@ -10754,7 +10751,7 @@
         <v>117</v>
       </c>
       <c r="L231" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="232" spans="1:12" x14ac:dyDescent="0.2">
@@ -10762,37 +10759,37 @@
         <v>458</v>
       </c>
       <c r="B232" t="s">
-        <v>39</v>
-      </c>
-      <c r="C232" t="s">
-        <v>121</v>
+        <v>38</v>
+      </c>
+      <c r="C232">
+        <v>1</v>
       </c>
       <c r="D232" t="s">
-        <v>245</v>
+        <v>23</v>
       </c>
       <c r="E232" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="F232" t="s">
         <v>11</v>
       </c>
       <c r="G232" t="s">
+        <v>249</v>
+      </c>
+      <c r="H232" t="s">
+        <v>35</v>
+      </c>
+      <c r="I232" t="s">
         <v>459</v>
       </c>
-      <c r="H232" t="s">
-        <v>13</v>
-      </c>
-      <c r="I232" t="s">
-        <v>176</v>
-      </c>
       <c r="J232" t="s">
-        <v>125</v>
+        <v>71</v>
       </c>
       <c r="K232" t="s">
         <v>117</v>
       </c>
       <c r="L232" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="233" spans="1:12" x14ac:dyDescent="0.2">
@@ -10802,43 +10799,43 @@
       <c r="B233" t="s">
         <v>38</v>
       </c>
-      <c r="C233">
-        <v>1</v>
+      <c r="C233" t="s">
+        <v>56</v>
       </c>
       <c r="D233" t="s">
-        <v>23</v>
+        <v>121</v>
       </c>
       <c r="E233" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="F233" t="s">
         <v>11</v>
       </c>
       <c r="G233" t="s">
-        <v>249</v>
+        <v>457</v>
       </c>
       <c r="H233" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="I233" t="s">
-        <v>461</v>
+        <v>176</v>
       </c>
       <c r="J233" t="s">
-        <v>71</v>
+        <v>98</v>
       </c>
       <c r="K233" t="s">
         <v>117</v>
       </c>
       <c r="L233" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="234" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B234" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C234" t="s">
         <v>56</v>
@@ -10847,36 +10844,36 @@
         <v>121</v>
       </c>
       <c r="E234" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="F234" t="s">
         <v>11</v>
       </c>
       <c r="G234" t="s">
-        <v>459</v>
+        <v>418</v>
       </c>
       <c r="H234" t="s">
         <v>13</v>
       </c>
       <c r="I234" t="s">
-        <v>176</v>
+        <v>14</v>
       </c>
       <c r="J234" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="K234" t="s">
         <v>117</v>
       </c>
       <c r="L234" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="235" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B235" t="s">
-        <v>39</v>
+        <v>303</v>
       </c>
       <c r="C235" t="s">
         <v>56</v>
@@ -10885,19 +10882,19 @@
         <v>121</v>
       </c>
       <c r="E235" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="F235" t="s">
         <v>11</v>
       </c>
       <c r="G235" t="s">
-        <v>420</v>
+        <v>240</v>
       </c>
       <c r="H235" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="I235" t="s">
-        <v>14</v>
+        <v>434</v>
       </c>
       <c r="J235" t="s">
         <v>101</v>
@@ -10906,91 +10903,91 @@
         <v>117</v>
       </c>
       <c r="L235" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="236" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B236" t="s">
-        <v>303</v>
+        <v>55</v>
       </c>
       <c r="C236" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="D236" t="s">
-        <v>121</v>
+        <v>9</v>
       </c>
       <c r="E236" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="F236" t="s">
         <v>11</v>
       </c>
       <c r="G236" t="s">
-        <v>240</v>
+        <v>26</v>
       </c>
       <c r="H236" t="s">
         <v>32</v>
       </c>
       <c r="I236" t="s">
-        <v>436</v>
+        <v>205</v>
       </c>
       <c r="J236" t="s">
-        <v>101</v>
+        <v>203</v>
       </c>
       <c r="K236" t="s">
         <v>117</v>
       </c>
       <c r="L236" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="237" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B237" t="s">
-        <v>55</v>
+        <v>158</v>
       </c>
       <c r="C237" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="D237" t="s">
-        <v>9</v>
+        <v>121</v>
       </c>
       <c r="E237" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="F237" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G237" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="H237" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="I237" t="s">
-        <v>205</v>
+        <v>14</v>
       </c>
       <c r="J237" t="s">
-        <v>203</v>
+        <v>65</v>
       </c>
       <c r="K237" t="s">
         <v>117</v>
       </c>
       <c r="L237" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="238" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B238" t="s">
-        <v>158</v>
+        <v>230</v>
       </c>
       <c r="C238" t="s">
         <v>56</v>
@@ -11002,80 +10999,80 @@
         <v>34</v>
       </c>
       <c r="F238" t="s">
-        <v>18</v>
+        <v>61</v>
       </c>
       <c r="G238" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H238" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="I238" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="J238" t="s">
-        <v>65</v>
+        <v>340</v>
       </c>
       <c r="K238" t="s">
         <v>117</v>
       </c>
       <c r="L238" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="239" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B239" t="s">
-        <v>230</v>
+        <v>272</v>
       </c>
       <c r="C239" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="D239" t="s">
-        <v>121</v>
+        <v>213</v>
       </c>
       <c r="E239" t="s">
-        <v>34</v>
+        <v>173</v>
       </c>
       <c r="F239" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="G239" t="s">
-        <v>57</v>
+        <v>249</v>
       </c>
       <c r="H239" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="I239" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="J239" t="s">
-        <v>340</v>
+        <v>101</v>
       </c>
       <c r="K239" t="s">
         <v>117</v>
       </c>
       <c r="L239" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="240" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B240" t="s">
-        <v>272</v>
+        <v>124</v>
       </c>
       <c r="C240" t="s">
-        <v>9</v>
+        <v>105</v>
       </c>
       <c r="D240" t="s">
-        <v>213</v>
+        <v>417</v>
       </c>
       <c r="E240" t="s">
-        <v>173</v>
+        <v>17</v>
       </c>
       <c r="F240" t="s">
         <v>11</v>
@@ -11084,48 +11081,48 @@
         <v>249</v>
       </c>
       <c r="H240" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="I240" t="s">
-        <v>37</v>
+        <v>419</v>
       </c>
       <c r="J240" t="s">
-        <v>101</v>
+        <v>65</v>
       </c>
       <c r="K240" t="s">
         <v>117</v>
       </c>
       <c r="L240" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="241" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B241" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C241" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="D241" t="s">
-        <v>419</v>
+        <v>114</v>
       </c>
       <c r="E241" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="F241" t="s">
         <v>11</v>
       </c>
       <c r="G241" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="H241" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="I241" t="s">
-        <v>421</v>
+        <v>116</v>
       </c>
       <c r="J241" t="s">
         <v>65</v>
@@ -11134,83 +11131,83 @@
         <v>117</v>
       </c>
       <c r="L241" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="242" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B242" t="s">
-        <v>120</v>
+        <v>22</v>
       </c>
       <c r="C242" t="s">
-        <v>113</v>
+        <v>11</v>
       </c>
       <c r="D242" t="s">
-        <v>114</v>
+        <v>11</v>
       </c>
       <c r="E242" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="F242" t="s">
         <v>11</v>
       </c>
       <c r="G242" t="s">
-        <v>240</v>
+        <v>11</v>
       </c>
       <c r="H242" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="I242" t="s">
-        <v>116</v>
+        <v>11</v>
       </c>
       <c r="J242" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="K242" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="L242" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="243" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
+        <v>470</v>
+      </c>
+      <c r="B243" t="s">
+        <v>7</v>
+      </c>
+      <c r="C243" t="s">
+        <v>16</v>
+      </c>
+      <c r="D243" t="s">
+        <v>8</v>
+      </c>
+      <c r="E243" t="s">
+        <v>10</v>
+      </c>
+      <c r="F243" t="s">
+        <v>18</v>
+      </c>
+      <c r="G243" t="s">
+        <v>26</v>
+      </c>
+      <c r="H243" t="s">
+        <v>13</v>
+      </c>
+      <c r="I243" t="s">
         <v>471</v>
       </c>
-      <c r="B243" t="s">
-        <v>22</v>
-      </c>
-      <c r="C243" t="s">
-        <v>11</v>
-      </c>
-      <c r="D243" t="s">
-        <v>11</v>
-      </c>
-      <c r="E243" t="s">
-        <v>11</v>
-      </c>
-      <c r="F243" t="s">
-        <v>11</v>
-      </c>
-      <c r="G243" t="s">
-        <v>11</v>
-      </c>
-      <c r="H243" t="s">
-        <v>11</v>
-      </c>
-      <c r="I243" t="s">
-        <v>11</v>
-      </c>
       <c r="J243" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="K243" t="s">
         <v>139</v>
       </c>
       <c r="L243" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="244" spans="1:12" x14ac:dyDescent="0.2">
@@ -11218,7 +11215,7 @@
         <v>472</v>
       </c>
       <c r="B244" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="C244" t="s">
         <v>16</v>
@@ -11236,65 +11233,65 @@
         <v>26</v>
       </c>
       <c r="H244" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="I244" t="s">
-        <v>473</v>
+        <v>37</v>
       </c>
       <c r="J244" t="s">
-        <v>65</v>
+        <v>203</v>
       </c>
       <c r="K244" t="s">
         <v>139</v>
       </c>
       <c r="L244" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="245" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B245" t="s">
-        <v>38</v>
+        <v>179</v>
       </c>
       <c r="C245" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D245" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E245" t="s">
         <v>10</v>
       </c>
       <c r="F245" t="s">
-        <v>18</v>
+        <v>134</v>
       </c>
       <c r="G245" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="H245" t="s">
-        <v>60</v>
+        <v>13</v>
       </c>
       <c r="I245" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="J245" t="s">
-        <v>203</v>
+        <v>71</v>
       </c>
       <c r="K245" t="s">
         <v>139</v>
       </c>
       <c r="L245" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="246" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B246" t="s">
-        <v>179</v>
+        <v>120</v>
       </c>
       <c r="C246" t="s">
         <v>8</v>
@@ -11303,28 +11300,28 @@
         <v>9</v>
       </c>
       <c r="E246" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="F246" t="s">
-        <v>134</v>
+        <v>475</v>
       </c>
       <c r="G246" t="s">
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="H246" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="I246" t="s">
         <v>11</v>
       </c>
       <c r="J246" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="K246" t="s">
         <v>139</v>
       </c>
       <c r="L246" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="247" spans="1:12" x14ac:dyDescent="0.2">
@@ -11332,22 +11329,22 @@
         <v>476</v>
       </c>
       <c r="B247" t="s">
-        <v>120</v>
+        <v>293</v>
       </c>
       <c r="C247" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="D247" t="s">
-        <v>9</v>
+        <v>121</v>
       </c>
       <c r="E247" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="F247" t="s">
-        <v>477</v>
+        <v>122</v>
       </c>
       <c r="G247" t="s">
-        <v>26</v>
+        <v>240</v>
       </c>
       <c r="H247" t="s">
         <v>35</v>
@@ -11356,36 +11353,36 @@
         <v>11</v>
       </c>
       <c r="J247" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="K247" t="s">
         <v>139</v>
       </c>
       <c r="L247" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="248" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
+        <v>477</v>
+      </c>
+      <c r="B248" t="s">
         <v>478</v>
       </c>
-      <c r="B248" t="s">
-        <v>293</v>
-      </c>
       <c r="C248" t="s">
+        <v>9</v>
+      </c>
+      <c r="D248" t="s">
         <v>56</v>
-      </c>
-      <c r="D248" t="s">
-        <v>121</v>
       </c>
       <c r="E248" t="s">
         <v>17</v>
       </c>
       <c r="F248" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="G248" t="s">
-        <v>240</v>
+        <v>59</v>
       </c>
       <c r="H248" t="s">
         <v>35</v>
@@ -11400,7 +11397,7 @@
         <v>139</v>
       </c>
       <c r="L248" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="249" spans="1:12" x14ac:dyDescent="0.2">
@@ -11408,7 +11405,7 @@
         <v>479</v>
       </c>
       <c r="B249" t="s">
-        <v>480</v>
+        <v>290</v>
       </c>
       <c r="C249" t="s">
         <v>9</v>
@@ -11423,7 +11420,7 @@
         <v>128</v>
       </c>
       <c r="G249" t="s">
-        <v>59</v>
+        <v>480</v>
       </c>
       <c r="H249" t="s">
         <v>35</v>
@@ -11432,13 +11429,13 @@
         <v>11</v>
       </c>
       <c r="J249" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="K249" t="s">
         <v>139</v>
       </c>
       <c r="L249" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="250" spans="1:12" x14ac:dyDescent="0.2">
@@ -11446,22 +11443,22 @@
         <v>481</v>
       </c>
       <c r="B250" t="s">
-        <v>290</v>
+        <v>124</v>
       </c>
       <c r="C250" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D250" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="E250" t="s">
         <v>17</v>
       </c>
       <c r="F250" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="G250" t="s">
-        <v>482</v>
+        <v>26</v>
       </c>
       <c r="H250" t="s">
         <v>35</v>
@@ -11470,112 +11467,112 @@
         <v>11</v>
       </c>
       <c r="J250" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="K250" t="s">
         <v>139</v>
       </c>
       <c r="L250" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="251" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B251" t="s">
-        <v>124</v>
+        <v>247</v>
       </c>
       <c r="C251" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D251" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E251" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F251" t="s">
         <v>134</v>
       </c>
       <c r="G251" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="H251" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="I251" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="J251" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="K251" t="s">
         <v>139</v>
       </c>
       <c r="L251" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="252" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B252" t="s">
-        <v>247</v>
+        <v>293</v>
       </c>
       <c r="C252" t="s">
-        <v>11</v>
+        <v>56</v>
       </c>
       <c r="D252" t="s">
-        <v>11</v>
+        <v>121</v>
       </c>
       <c r="E252" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F252" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="G252" t="s">
-        <v>57</v>
+        <v>240</v>
       </c>
       <c r="H252" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="I252" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="J252" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="K252" t="s">
         <v>139</v>
       </c>
       <c r="L252" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="253" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B253" t="s">
-        <v>293</v>
+        <v>478</v>
       </c>
       <c r="C253" t="s">
+        <v>9</v>
+      </c>
+      <c r="D253" t="s">
         <v>56</v>
-      </c>
-      <c r="D253" t="s">
-        <v>121</v>
       </c>
       <c r="E253" t="s">
         <v>17</v>
       </c>
       <c r="F253" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="G253" t="s">
-        <v>240</v>
+        <v>59</v>
       </c>
       <c r="H253" t="s">
         <v>35</v>
@@ -11590,121 +11587,121 @@
         <v>139</v>
       </c>
       <c r="L253" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="254" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B254" t="s">
-        <v>480</v>
+        <v>158</v>
       </c>
       <c r="C254" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D254" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="E254" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F254" t="s">
-        <v>128</v>
+        <v>61</v>
       </c>
       <c r="G254" t="s">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="H254" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="I254" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="J254" t="s">
-        <v>65</v>
+        <v>101</v>
       </c>
       <c r="K254" t="s">
         <v>139</v>
       </c>
       <c r="L254" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="255" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B255" t="s">
-        <v>158</v>
+        <v>36</v>
       </c>
       <c r="C255" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D255" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E255" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F255" t="s">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="G255" t="s">
-        <v>12</v>
+        <v>237</v>
       </c>
       <c r="H255" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="I255" t="s">
-        <v>14</v>
+        <v>97</v>
       </c>
       <c r="J255" t="s">
-        <v>101</v>
+        <v>72</v>
       </c>
       <c r="K255" t="s">
         <v>139</v>
       </c>
       <c r="L255" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="256" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
+        <v>487</v>
+      </c>
+      <c r="B256" t="s">
         <v>488</v>
       </c>
-      <c r="B256" t="s">
-        <v>36</v>
-      </c>
       <c r="C256" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="D256" t="s">
-        <v>9</v>
+        <v>245</v>
       </c>
       <c r="E256" t="s">
-        <v>10</v>
+        <v>423</v>
       </c>
       <c r="F256" t="s">
-        <v>18</v>
+        <v>128</v>
       </c>
       <c r="G256" t="s">
-        <v>237</v>
+        <v>383</v>
       </c>
       <c r="H256" t="s">
         <v>35</v>
       </c>
       <c r="I256" t="s">
-        <v>97</v>
+        <v>11</v>
       </c>
       <c r="J256" t="s">
-        <v>72</v>
+        <v>101</v>
       </c>
       <c r="K256" t="s">
         <v>139</v>
       </c>
       <c r="L256" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="257" spans="1:12" x14ac:dyDescent="0.2">
@@ -11712,28 +11709,28 @@
         <v>489</v>
       </c>
       <c r="B257" t="s">
-        <v>490</v>
+        <v>127</v>
       </c>
       <c r="C257" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="D257" t="s">
-        <v>245</v>
+        <v>9</v>
       </c>
       <c r="E257" t="s">
-        <v>425</v>
+        <v>79</v>
       </c>
       <c r="F257" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="G257" t="s">
-        <v>384</v>
+        <v>54</v>
       </c>
       <c r="H257" t="s">
         <v>35</v>
       </c>
       <c r="I257" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="J257" t="s">
         <v>101</v>
@@ -11742,53 +11739,53 @@
         <v>139</v>
       </c>
       <c r="L257" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="258" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B258" t="s">
-        <v>127</v>
+        <v>29</v>
       </c>
       <c r="C258" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D258" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E258" t="s">
-        <v>79</v>
+        <v>11</v>
       </c>
       <c r="F258" t="s">
-        <v>134</v>
+        <v>11</v>
       </c>
       <c r="G258" t="s">
-        <v>54</v>
+        <v>148</v>
       </c>
       <c r="H258" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="I258" t="s">
         <v>14</v>
       </c>
       <c r="J258" t="s">
-        <v>101</v>
+        <v>71</v>
       </c>
       <c r="K258" t="s">
         <v>139</v>
       </c>
       <c r="L258" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="259" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B259" t="s">
-        <v>29</v>
+        <v>221</v>
       </c>
       <c r="C259" t="s">
         <v>11</v>
@@ -11800,39 +11797,39 @@
         <v>11</v>
       </c>
       <c r="F259" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G259" t="s">
-        <v>148</v>
+        <v>59</v>
       </c>
       <c r="H259" t="s">
         <v>11</v>
       </c>
       <c r="I259" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="J259" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="K259" t="s">
         <v>139</v>
       </c>
       <c r="L259" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="260" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B260" t="s">
-        <v>221</v>
+        <v>303</v>
       </c>
       <c r="C260" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D260" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E260" t="s">
         <v>11</v>
@@ -11841,22 +11838,22 @@
         <v>18</v>
       </c>
       <c r="G260" t="s">
-        <v>59</v>
+        <v>249</v>
       </c>
       <c r="H260" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="I260" t="s">
-        <v>11</v>
+        <v>493</v>
       </c>
       <c r="J260" t="s">
-        <v>65</v>
+        <v>125</v>
       </c>
       <c r="K260" t="s">
         <v>139</v>
       </c>
       <c r="L260" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="261" spans="1:12" x14ac:dyDescent="0.2">
@@ -11864,60 +11861,60 @@
         <v>494</v>
       </c>
       <c r="B261" t="s">
-        <v>303</v>
+        <v>247</v>
       </c>
       <c r="C261" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D261" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E261" t="s">
-        <v>11</v>
+        <v>390</v>
       </c>
       <c r="F261" t="s">
-        <v>18</v>
+        <v>304</v>
       </c>
       <c r="G261" t="s">
-        <v>249</v>
+        <v>57</v>
       </c>
       <c r="H261" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="I261" t="s">
-        <v>495</v>
+        <v>11</v>
       </c>
       <c r="J261" t="s">
-        <v>125</v>
+        <v>340</v>
       </c>
       <c r="K261" t="s">
         <v>139</v>
       </c>
       <c r="L261" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="262" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B262" t="s">
-        <v>247</v>
+        <v>120</v>
       </c>
       <c r="C262" t="s">
+        <v>16</v>
+      </c>
+      <c r="D262" t="s">
         <v>8</v>
       </c>
-      <c r="D262" t="s">
-        <v>9</v>
-      </c>
       <c r="E262" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F262" t="s">
-        <v>304</v>
+        <v>475</v>
       </c>
       <c r="G262" t="s">
-        <v>57</v>
+        <v>12</v>
       </c>
       <c r="H262" t="s">
         <v>13</v>
@@ -11932,45 +11929,45 @@
         <v>139</v>
       </c>
       <c r="L262" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="263" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
+        <v>496</v>
+      </c>
+      <c r="B263" t="s">
         <v>497</v>
       </c>
-      <c r="B263" t="s">
-        <v>120</v>
-      </c>
       <c r="C263" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D263" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E263" t="s">
-        <v>391</v>
+        <v>10</v>
       </c>
       <c r="F263" t="s">
-        <v>477</v>
+        <v>61</v>
       </c>
       <c r="G263" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H263" t="s">
         <v>13</v>
       </c>
       <c r="I263" t="s">
-        <v>11</v>
+        <v>337</v>
       </c>
       <c r="J263" t="s">
-        <v>340</v>
+        <v>170</v>
       </c>
       <c r="K263" t="s">
         <v>139</v>
       </c>
       <c r="L263" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="264" spans="1:12" x14ac:dyDescent="0.2">
@@ -11978,7 +11975,7 @@
         <v>498</v>
       </c>
       <c r="B264" t="s">
-        <v>499</v>
+        <v>127</v>
       </c>
       <c r="C264" t="s">
         <v>8</v>
@@ -11990,25 +11987,25 @@
         <v>10</v>
       </c>
       <c r="F264" t="s">
-        <v>61</v>
+        <v>134</v>
       </c>
       <c r="G264" t="s">
-        <v>11</v>
+        <v>54</v>
       </c>
       <c r="H264" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="I264" t="s">
-        <v>337</v>
+        <v>14</v>
       </c>
       <c r="J264" t="s">
-        <v>170</v>
+        <v>499</v>
       </c>
       <c r="K264" t="s">
         <v>139</v>
       </c>
       <c r="L264" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="265" spans="1:12" x14ac:dyDescent="0.2">
@@ -12016,66 +12013,66 @@
         <v>500</v>
       </c>
       <c r="B265" t="s">
-        <v>127</v>
-      </c>
-      <c r="C265" t="s">
-        <v>8</v>
+        <v>22</v>
+      </c>
+      <c r="C265">
+        <v>1</v>
       </c>
       <c r="D265" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="E265" t="s">
         <v>10</v>
       </c>
       <c r="F265" t="s">
-        <v>134</v>
+        <v>18</v>
       </c>
       <c r="G265" t="s">
-        <v>54</v>
+        <v>501</v>
       </c>
       <c r="H265" t="s">
         <v>35</v>
       </c>
       <c r="I265" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="J265" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="K265" t="s">
         <v>139</v>
       </c>
       <c r="L265" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="266" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="B266" t="s">
-        <v>22</v>
-      </c>
-      <c r="C266">
-        <v>1</v>
+        <v>31</v>
+      </c>
+      <c r="C266" t="s">
+        <v>16</v>
       </c>
       <c r="D266" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="E266" t="s">
         <v>10</v>
       </c>
       <c r="F266" t="s">
-        <v>18</v>
+        <v>136</v>
       </c>
       <c r="G266" t="s">
-        <v>503</v>
+        <v>19</v>
       </c>
       <c r="H266" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="I266" t="s">
-        <v>73</v>
+        <v>429</v>
       </c>
       <c r="J266" t="s">
         <v>504</v>
@@ -12084,7 +12081,7 @@
         <v>139</v>
       </c>
       <c r="L266" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="267" spans="1:12" x14ac:dyDescent="0.2">
@@ -12092,7 +12089,7 @@
         <v>505</v>
       </c>
       <c r="B267" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="C267" t="s">
         <v>16</v>
@@ -12107,45 +12104,45 @@
         <v>136</v>
       </c>
       <c r="G267" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="H267" t="s">
         <v>13</v>
       </c>
       <c r="I267" t="s">
-        <v>431</v>
+        <v>11</v>
       </c>
       <c r="J267" t="s">
-        <v>506</v>
+        <v>87</v>
       </c>
       <c r="K267" t="s">
         <v>139</v>
       </c>
       <c r="L267" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="268" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B268" t="s">
-        <v>7</v>
+        <v>221</v>
       </c>
       <c r="C268" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D268" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="E268" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="F268" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G268" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="H268" t="s">
         <v>13</v>
@@ -12154,112 +12151,112 @@
         <v>11</v>
       </c>
       <c r="J268" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="K268" t="s">
         <v>139</v>
       </c>
       <c r="L268" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="269" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B269" t="s">
-        <v>221</v>
+        <v>11</v>
       </c>
       <c r="C269" t="s">
+        <v>8</v>
+      </c>
+      <c r="D269" t="s">
         <v>9</v>
       </c>
-      <c r="D269" t="s">
-        <v>56</v>
-      </c>
       <c r="E269" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="F269" t="s">
-        <v>128</v>
+        <v>11</v>
       </c>
       <c r="G269" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
       <c r="H269" t="s">
         <v>13</v>
       </c>
       <c r="I269" t="s">
-        <v>11</v>
+        <v>205</v>
       </c>
       <c r="J269" t="s">
-        <v>65</v>
+        <v>504</v>
       </c>
       <c r="K269" t="s">
         <v>139</v>
       </c>
       <c r="L269" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="270" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B270" t="s">
-        <v>11</v>
+        <v>287</v>
       </c>
       <c r="C270" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D270" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E270" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F270" t="s">
-        <v>11</v>
+        <v>61</v>
       </c>
       <c r="G270" t="s">
         <v>19</v>
       </c>
       <c r="H270" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="I270" t="s">
-        <v>205</v>
+        <v>11</v>
       </c>
       <c r="J270" t="s">
-        <v>506</v>
+        <v>84</v>
       </c>
       <c r="K270" t="s">
         <v>139</v>
       </c>
       <c r="L270" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="271" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
+        <v>509</v>
+      </c>
+      <c r="B271" t="s">
+        <v>478</v>
+      </c>
+      <c r="C271" t="s">
+        <v>16</v>
+      </c>
+      <c r="D271" t="s">
+        <v>8</v>
+      </c>
+      <c r="E271" t="s">
         <v>510</v>
       </c>
-      <c r="B271" t="s">
-        <v>287</v>
-      </c>
-      <c r="C271" t="s">
-        <v>11</v>
-      </c>
-      <c r="D271" t="s">
-        <v>11</v>
-      </c>
-      <c r="E271" t="s">
-        <v>11</v>
-      </c>
       <c r="F271" t="s">
-        <v>61</v>
+        <v>134</v>
       </c>
       <c r="G271" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="H271" t="s">
         <v>35</v>
@@ -12274,7 +12271,7 @@
         <v>139</v>
       </c>
       <c r="L271" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="272" spans="1:12" x14ac:dyDescent="0.2">
@@ -12282,42 +12279,42 @@
         <v>511</v>
       </c>
       <c r="B272" t="s">
-        <v>480</v>
+        <v>22</v>
       </c>
       <c r="C272" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D272" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E272" t="s">
-        <v>512</v>
+        <v>11</v>
       </c>
       <c r="F272" t="s">
-        <v>134</v>
+        <v>11</v>
       </c>
       <c r="G272" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="H272" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="I272" t="s">
         <v>11</v>
       </c>
       <c r="J272" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="K272" t="s">
-        <v>139</v>
+        <v>153</v>
       </c>
       <c r="L272" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="273" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B273" t="s">
         <v>22</v>
@@ -12350,21 +12347,21 @@
         <v>153</v>
       </c>
       <c r="L273" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="274" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
+        <v>513</v>
+      </c>
+      <c r="B274" t="s">
         <v>514</v>
       </c>
-      <c r="B274" t="s">
-        <v>22</v>
-      </c>
-      <c r="C274" t="s">
-        <v>11</v>
-      </c>
-      <c r="D274" t="s">
-        <v>11</v>
+      <c r="C274">
+        <v>1</v>
+      </c>
+      <c r="D274">
+        <v>1</v>
       </c>
       <c r="E274" t="s">
         <v>11</v>
@@ -12373,22 +12370,22 @@
         <v>11</v>
       </c>
       <c r="G274" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="H274" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I274" t="s">
-        <v>11</v>
+        <v>67</v>
       </c>
       <c r="J274" t="s">
-        <v>65</v>
+        <v>504</v>
       </c>
       <c r="K274" t="s">
         <v>153</v>
       </c>
       <c r="L274" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="275" spans="1:12" x14ac:dyDescent="0.2">
@@ -12396,13 +12393,13 @@
         <v>515</v>
       </c>
       <c r="B275" t="s">
-        <v>516</v>
-      </c>
-      <c r="C275">
-        <v>1</v>
-      </c>
-      <c r="D275">
-        <v>1</v>
+        <v>22</v>
+      </c>
+      <c r="C275" t="s">
+        <v>16</v>
+      </c>
+      <c r="D275" t="s">
+        <v>8</v>
       </c>
       <c r="E275" t="s">
         <v>11</v>
@@ -12411,36 +12408,36 @@
         <v>11</v>
       </c>
       <c r="G275" t="s">
-        <v>26</v>
+        <v>148</v>
       </c>
       <c r="H275" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="I275" t="s">
-        <v>67</v>
+        <v>11</v>
       </c>
       <c r="J275" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="K275" t="s">
         <v>153</v>
       </c>
       <c r="L275" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="276" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B276" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C276" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D276" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E276" t="s">
         <v>11</v>
@@ -12449,30 +12446,30 @@
         <v>11</v>
       </c>
       <c r="G276" t="s">
-        <v>148</v>
+        <v>12</v>
       </c>
       <c r="H276" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="I276" t="s">
-        <v>11</v>
+        <v>67</v>
       </c>
       <c r="J276" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="K276" t="s">
         <v>153</v>
       </c>
       <c r="L276" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="277" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B277" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C277" t="s">
         <v>11</v>
@@ -12487,98 +12484,60 @@
         <v>11</v>
       </c>
       <c r="G277" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="H277" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="I277" t="s">
-        <v>67</v>
+        <v>11</v>
       </c>
       <c r="J277" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="K277" t="s">
         <v>153</v>
       </c>
       <c r="L277" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="278" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
+        <v>518</v>
+      </c>
+      <c r="B278" t="s">
+        <v>22</v>
+      </c>
+      <c r="C278" t="s">
+        <v>11</v>
+      </c>
+      <c r="D278" t="s">
+        <v>11</v>
+      </c>
+      <c r="E278" t="s">
+        <v>11</v>
+      </c>
+      <c r="F278" t="s">
+        <v>11</v>
+      </c>
+      <c r="G278" t="s">
+        <v>19</v>
+      </c>
+      <c r="H278" t="s">
+        <v>11</v>
+      </c>
+      <c r="I278" t="s">
+        <v>11</v>
+      </c>
+      <c r="J278" t="s">
         <v>519</v>
-      </c>
-      <c r="B278" t="s">
-        <v>31</v>
-      </c>
-      <c r="C278" t="s">
-        <v>11</v>
-      </c>
-      <c r="D278" t="s">
-        <v>11</v>
-      </c>
-      <c r="E278" t="s">
-        <v>11</v>
-      </c>
-      <c r="F278" t="s">
-        <v>11</v>
-      </c>
-      <c r="G278" t="s">
-        <v>26</v>
-      </c>
-      <c r="H278" t="s">
-        <v>35</v>
-      </c>
-      <c r="I278" t="s">
-        <v>11</v>
-      </c>
-      <c r="J278" t="s">
-        <v>506</v>
       </c>
       <c r="K278" t="s">
         <v>153</v>
       </c>
       <c r="L278" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="279" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A279" t="s">
         <v>520</v>
-      </c>
-      <c r="B279" t="s">
-        <v>22</v>
-      </c>
-      <c r="C279" t="s">
-        <v>11</v>
-      </c>
-      <c r="D279" t="s">
-        <v>11</v>
-      </c>
-      <c r="E279" t="s">
-        <v>11</v>
-      </c>
-      <c r="F279" t="s">
-        <v>11</v>
-      </c>
-      <c r="G279" t="s">
-        <v>19</v>
-      </c>
-      <c r="H279" t="s">
-        <v>11</v>
-      </c>
-      <c r="I279" t="s">
-        <v>11</v>
-      </c>
-      <c r="J279" t="s">
-        <v>521</v>
-      </c>
-      <c r="K279" t="s">
-        <v>153</v>
-      </c>
-      <c r="L279" t="s">
-        <v>522</v>
       </c>
     </row>
   </sheetData>

</xml_diff>